<commit_message>
armando interface para compras
</commit_message>
<xml_diff>
--- a/contable_detalle.xlsx
+++ b/contable_detalle.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master Kaizen - MK\Documents\NetBeansProjects\contable01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{820D161B-315B-4150-918C-5D605FE72A15}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="db_cliente" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="db_plan" sheetId="5" r:id="rId2"/>
+    <sheet name="db_compras" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Columna</t>
   </si>
@@ -55,12 +51,132 @@
   </si>
   <si>
     <t>C = Cliente P = Proveedor</t>
+  </si>
+  <si>
+    <t>cuenta</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>serie</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>cargo</t>
+  </si>
+  <si>
+    <t>abono</t>
+  </si>
+  <si>
+    <t>mercad</t>
+  </si>
+  <si>
+    <t>base imponible GRAVADAS</t>
+  </si>
+  <si>
+    <t>IGV GRAVADAS</t>
+  </si>
+  <si>
+    <t>base imponible GRAVADAS PARA NO GRAVADAS</t>
+  </si>
+  <si>
+    <t>IGV GRAVADAS PARA NO GRAVADAS</t>
+  </si>
+  <si>
+    <t>Valor de adquisiciones NO GRAVADAS</t>
+  </si>
+  <si>
+    <t>IMPORTE TOTAL</t>
+  </si>
+  <si>
+    <t>94 costos y gastos</t>
+  </si>
+  <si>
+    <t>95 costos y gastos</t>
+  </si>
+  <si>
+    <t>Codigo contable para forma de pago</t>
+  </si>
+  <si>
+    <t>asiento en diario</t>
+  </si>
+  <si>
+    <t>correlativo</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a13</t>
+  </si>
+  <si>
+    <t>a14</t>
+  </si>
+  <si>
+    <t>a15</t>
+  </si>
+  <si>
+    <t>a16</t>
+  </si>
+  <si>
+    <t>a17</t>
+  </si>
+  <si>
+    <t>a18</t>
+  </si>
+  <si>
+    <t>a19</t>
+  </si>
+  <si>
+    <t>a20</t>
+  </si>
+  <si>
+    <t>a21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -115,16 +231,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,26 +346,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,23 +381,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,10 +556,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -568,7 +663,418 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>500</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja3"/>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>200</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>200</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -579,8 +1085,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
interfaces compra y venta, falta nombre de elementos compra
</commit_message>
<xml_diff>
--- a/contable_detalle.xlsx
+++ b/contable_detalle.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master Kaizen - MK\Documents\NetBeansProjects\contable01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A5FAF033-89A1-43C5-A682-91ADEB7B4995}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_cliente" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
   <si>
     <t>Columna</t>
   </si>
@@ -171,12 +177,90 @@
   </si>
   <si>
     <t>a21</t>
+  </si>
+  <si>
+    <t>Fecha de Emision</t>
+  </si>
+  <si>
+    <t>Fecha de Vencimiento</t>
+  </si>
+  <si>
+    <t>TIPO (tabla 10)</t>
+  </si>
+  <si>
+    <t>Serie</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>TIPO (tabla 2)</t>
+  </si>
+  <si>
+    <t>DOCUMENTO DE IDENTIDAD</t>
+  </si>
+  <si>
+    <t>COMPROBANTE DE PAGO</t>
+  </si>
+  <si>
+    <t>Apellidos y nombres</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Abono</t>
+  </si>
+  <si>
+    <t>COD. CONTABLE</t>
+  </si>
+  <si>
+    <t>Valor facturado de la exportacion</t>
+  </si>
+  <si>
+    <t>Base imponible de la operación gravada</t>
+  </si>
+  <si>
+    <t>Exonerada</t>
+  </si>
+  <si>
+    <t>Inafecta</t>
+  </si>
+  <si>
+    <t>Importe de la operación exonerada o inafecta</t>
+  </si>
+  <si>
+    <t>ISC</t>
+  </si>
+  <si>
+    <t>IGV o IPM</t>
+  </si>
+  <si>
+    <t>Otros tributos y cargos que no forman parte de la base imponible</t>
+  </si>
+  <si>
+    <t>Importe total del comprobante de pago</t>
+  </si>
+  <si>
+    <t>Tipo de cambio</t>
+  </si>
+  <si>
+    <t>COD CTA OPERACIÓN AL CONTADO</t>
+  </si>
+  <si>
+    <t>Asiento</t>
+  </si>
+  <si>
+    <t>a22</t>
+  </si>
+  <si>
+    <t>a23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,13 +330,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,9 +433,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,6 +485,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -556,7 +677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -663,7 +784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -742,12 +863,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,20 +1194,366 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E16:E17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>